<commit_message>
Cambio en llave primaria de NIT por codigoEntidad y se permite la carga multiples veces de archivo entidades
</commit_message>
<xml_diff>
--- a/Proyecto Pago Seguridad Social/django_project_pss/media/datos_entidades.xlsx
+++ b/Proyecto Pago Seguridad Social/django_project_pss/media/datos_entidades.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20340"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naguie\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naguie\OneDrive - Consejo Superior de la Judicatura\Aplicativo Seguridad Social\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="28" documentId="11_58D71E6630CDE0943FFC9119BE7F6DF70EDA2F66" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1159AE30-B8F9-4E2F-B69B-7DEFC61523F2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datos Entidades" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
   <si>
     <t>NIT</t>
   </si>
@@ -216,12 +217,15 @@
   </si>
   <si>
     <t>COD</t>
+  </si>
+  <si>
+    <t>ESSC24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -565,18 +569,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.85546875" style="2"/>
-    <col min="2" max="2" width="21.85546875" style="5"/>
-    <col min="3" max="7" width="21.85546875" style="2"/>
+    <col min="2" max="2" width="21.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="2" customWidth="1"/>
+    <col min="4" max="7" width="21.85546875" style="2"/>
     <col min="8" max="8" width="21.85546875" style="2" customWidth="1"/>
     <col min="9" max="16384" width="21.85546875" style="2"/>
   </cols>
@@ -898,7 +903,7 @@
         <v>900226715</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>13</v>
@@ -921,42 +926,42 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>900336004</v>
+        <v>900226715</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G14" s="2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H14" s="2">
-        <v>23001010201</v>
+        <v>23001010102</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>800229739</v>
-      </c>
-      <c r="B15" s="5">
-        <v>230201</v>
+        <v>900336004</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>14</v>
+      <c r="D15" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>10</v>
@@ -973,16 +978,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>800227940</v>
+        <v>800229739</v>
       </c>
       <c r="B16" s="5">
-        <v>231001</v>
+        <v>230201</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>12</v>
+      <c r="D16" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>10</v>
@@ -999,16 +1004,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>800224808</v>
+        <v>800227940</v>
       </c>
       <c r="B17" s="5">
-        <v>230301</v>
+        <v>231001</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>10</v>
@@ -1025,157 +1030,183 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>860011153</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>57</v>
+        <v>800224808</v>
+      </c>
+      <c r="B18" s="5">
+        <v>230301</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="G18" s="2">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="H18" s="2">
-        <v>23001010301</v>
+        <v>23001010201</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>891480000</v>
+        <v>860011153</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G19" s="2">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="H19" s="2">
-        <v>23001010401</v>
+        <v>23001010301</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>899999239</v>
+        <v>891480000</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G20" s="2">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H20" s="2">
-        <v>230010108</v>
+        <v>23001010401</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>899999034</v>
+        <v>899999239</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G21" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H21" s="2">
-        <v>230010105</v>
+        <v>230010108</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>899999054</v>
+        <v>899999034</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G22" s="2">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="H22" s="2">
-        <v>230010106</v>
+        <v>230010105</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>899999001</v>
+        <v>899999054</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="2">
+        <v>72</v>
+      </c>
+      <c r="H23" s="2">
+        <v>230010106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>899999001</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G24" s="2">
         <v>90</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H24" s="2">
         <v>230010107</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Añade informacion de planilla a la bd
</commit_message>
<xml_diff>
--- a/Proyecto Pago Seguridad Social/django_project_pss/media/datos_entidades.xlsx
+++ b/Proyecto Pago Seguridad Social/django_project_pss/media/datos_entidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naguie\OneDrive - Consejo Superior de la Judicatura\Aplicativo Seguridad Social\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_58D71E6630CDE0943FFC9119BE7F6DF70EDA2F66" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1159AE30-B8F9-4E2F-B69B-7DEFC61523F2}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="11_58D71E6630CDE0943FFC9119BE7F6DF70EDA2F66" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1FBACD90-FF7D-49CA-8FDC-B49CB556F7DE}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,10 +216,10 @@
     <t>PAMIED</t>
   </si>
   <si>
-    <t>COD</t>
-  </si>
-  <si>
     <t>ESSC24</t>
+  </si>
+  <si>
+    <t>ESSC62</t>
   </si>
 </sst>
 </file>
@@ -773,7 +773,7 @@
         <v>900935126</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>13</v>
@@ -903,7 +903,7 @@
         <v>900226715</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Añade atributo tipo a la clase entidad
</commit_message>
<xml_diff>
--- a/Proyecto Pago Seguridad Social/django_project_pss/media/datos_entidades.xlsx
+++ b/Proyecto Pago Seguridad Social/django_project_pss/media/datos_entidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naguie\OneDrive - Consejo Superior de la Judicatura\Aplicativo Seguridad Social\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="11_58D71E6630CDE0943FFC9119BE7F6DF70EDA2F66" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1FBACD90-FF7D-49CA-8FDC-B49CB556F7DE}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="11_58D71E6630CDE0943FFC9119BE7F6DF70EDA2F66" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{9BA7EB6B-7F82-4439-9B9D-7E2CA6F74870}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="70">
   <si>
     <t>NIT</t>
   </si>
@@ -220,6 +220,21 @@
   </si>
   <si>
     <t>ESSC62</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>FONDOS PUBL. ADMINIST. PENSIONES</t>
+  </si>
+  <si>
+    <t>FONDOS PRIV. ADMINIST. PENSIONES</t>
+  </si>
+  <si>
+    <t>EMP. PRIV. PROMOTORAS DE SALUD</t>
+  </si>
+  <si>
+    <t>PARAFISCALES</t>
   </si>
 </sst>
 </file>
@@ -570,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -583,10 +598,11 @@
     <col min="3" max="3" width="21.85546875" style="2" customWidth="1"/>
     <col min="4" max="7" width="21.85546875" style="2"/>
     <col min="8" max="8" width="21.85546875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="21.85546875" style="2"/>
+    <col min="9" max="9" width="43.85546875" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="21.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,8 +627,11 @@
       <c r="H1" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>800088702</v>
       </c>
@@ -637,8 +656,11 @@
       <c r="H2" s="2">
         <v>23001010102</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>805001157</v>
       </c>
@@ -663,8 +685,11 @@
       <c r="H3" s="2">
         <v>23001010102</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>800130907</v>
       </c>
@@ -689,8 +714,11 @@
       <c r="H4" s="2">
         <v>23001010102</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>800251440</v>
       </c>
@@ -715,8 +743,11 @@
       <c r="H5" s="2">
         <v>23001010102</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>900156264</v>
       </c>
@@ -741,8 +772,11 @@
       <c r="H6" s="2">
         <v>23001010102</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>809008362</v>
       </c>
@@ -767,8 +801,11 @@
       <c r="H7" s="2">
         <v>23001010102</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>900935126</v>
       </c>
@@ -793,8 +830,11 @@
       <c r="H8" s="2">
         <v>23001010102</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>860066942</v>
       </c>
@@ -819,8 +859,11 @@
       <c r="H9" s="2">
         <v>23001010102</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>890303093</v>
       </c>
@@ -845,8 +888,11 @@
       <c r="H10" s="2">
         <v>23001010102</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>830003564</v>
       </c>
@@ -871,8 +917,11 @@
       <c r="H11" s="2">
         <v>23001010102</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>901037916</v>
       </c>
@@ -897,8 +946,11 @@
       <c r="H12" s="2">
         <v>23001010102</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>900226715</v>
       </c>
@@ -923,8 +975,11 @@
       <c r="H13" s="2">
         <v>23001010102</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>900226715</v>
       </c>
@@ -949,8 +1004,11 @@
       <c r="H14" s="2">
         <v>23001010102</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>900336004</v>
       </c>
@@ -975,8 +1033,11 @@
       <c r="H15" s="2">
         <v>23001010201</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>800229739</v>
       </c>
@@ -1001,8 +1062,11 @@
       <c r="H16" s="2">
         <v>23001010201</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>800227940</v>
       </c>
@@ -1027,8 +1091,11 @@
       <c r="H17" s="2">
         <v>23001010201</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>800224808</v>
       </c>
@@ -1053,8 +1120,11 @@
       <c r="H18" s="2">
         <v>23001010201</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>860011153</v>
       </c>
@@ -1079,8 +1149,11 @@
       <c r="H19" s="2">
         <v>23001010301</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>891480000</v>
       </c>
@@ -1105,8 +1178,11 @@
       <c r="H20" s="2">
         <v>23001010401</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>899999239</v>
       </c>
@@ -1131,8 +1207,11 @@
       <c r="H21" s="2">
         <v>230010108</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>899999034</v>
       </c>
@@ -1157,8 +1236,11 @@
       <c r="H22" s="2">
         <v>230010105</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>899999054</v>
       </c>
@@ -1183,8 +1265,11 @@
       <c r="H23" s="2">
         <v>230010106</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>899999001</v>
       </c>
@@ -1208,6 +1293,9 @@
       </c>
       <c r="H24" s="2">
         <v>230010107</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregan nuevas entidades de salud en documento y en reporte
</commit_message>
<xml_diff>
--- a/Proyecto Pago Seguridad Social/django_project_pss/media/datos_entidades.xlsx
+++ b/Proyecto Pago Seguridad Social/django_project_pss/media/datos_entidades.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naguie\OneDrive - Consejo Superior de la Judicatura\Aplicativo Seguridad Social\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="11_58D71E6630CDE0943FFC9119BE7F6DF70EDA2F66" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{9BA7EB6B-7F82-4439-9B9D-7E2CA6F74870}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="11_58D71E6630CDE0943FFC9119BE7F6DF70EDA2F66" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F65B40EC-32C2-43A4-8BBA-9D8CF4A0221C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datos Entidades" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'datos Entidades'!$A$1:$A$27</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="78">
   <si>
     <t>NIT</t>
   </si>
@@ -235,6 +238,30 @@
   </si>
   <si>
     <t>PARAFISCALES</t>
+  </si>
+  <si>
+    <t>MEDIMAS</t>
+  </si>
+  <si>
+    <t>COOMEVA</t>
+  </si>
+  <si>
+    <t>ASOCIACION MUTUAL EMSSANAR</t>
+  </si>
+  <si>
+    <t>CAFESALUD</t>
+  </si>
+  <si>
+    <t>COD1</t>
+  </si>
+  <si>
+    <t>COD2</t>
+  </si>
+  <si>
+    <t>COD3</t>
+  </si>
+  <si>
+    <t>COD4</t>
   </si>
 </sst>
 </file>
@@ -585,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1298,6 +1325,122 @@
         <v>69</v>
       </c>
     </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>901097473</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="2">
+        <v>73</v>
+      </c>
+      <c r="H25" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>805000427</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="2">
+        <v>73</v>
+      </c>
+      <c r="H26" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>814000337</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="2">
+        <v>73</v>
+      </c>
+      <c r="H27" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>800140949</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="2">
+        <v>73</v>
+      </c>
+      <c r="H28" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Se añade rubro temporal y permanente a patronales
</commit_message>
<xml_diff>
--- a/Proyecto Pago Seguridad Social/django_project_pss/media/datos_entidades.xlsx
+++ b/Proyecto Pago Seguridad Social/django_project_pss/media/datos_entidades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naguie\OneDrive - Consejo Superior de la Judicatura\Aplicativo Seguridad Social\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naguie\OneDrive - Consejo Superior de la Judicatura\RAMA JUDICIAL\Aplicativo Seguridad Social\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="11_58D71E6630CDE0943FFC9119BE7F6DF70EDA2F66" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F65B40EC-32C2-43A4-8BBA-9D8CF4A0221C}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="11_58D71E6630CDE0943FFC9119BE7F6DF70EDA2F66" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{84BED5ED-075E-43F4-BE79-CD88E14E632E}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="87">
   <si>
     <t>NIT</t>
   </si>
@@ -39,9 +39,6 @@
     <t>razonEntidad</t>
   </si>
   <si>
-    <t>rubro</t>
-  </si>
-  <si>
     <t>tipoCuentaPagar</t>
   </si>
   <si>
@@ -262,6 +259,36 @@
   </si>
   <si>
     <t>COD4</t>
+  </si>
+  <si>
+    <t>rubroPermanente</t>
+  </si>
+  <si>
+    <t>rubroTemporal</t>
+  </si>
+  <si>
+    <t>A010202002</t>
+  </si>
+  <si>
+    <t>A010202004</t>
+  </si>
+  <si>
+    <t>A010202005</t>
+  </si>
+  <si>
+    <t>A010202006</t>
+  </si>
+  <si>
+    <t>A010202007</t>
+  </si>
+  <si>
+    <t>A010202008</t>
+  </si>
+  <si>
+    <t>A010202009</t>
+  </si>
+  <si>
+    <t>A010202001</t>
   </si>
 </sst>
 </file>
@@ -612,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -623,21 +650,21 @@
     <col min="1" max="1" width="21.85546875" style="2"/>
     <col min="2" max="2" width="21.85546875" style="5" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" style="2" customWidth="1"/>
-    <col min="4" max="7" width="21.85546875" style="2"/>
-    <col min="8" max="8" width="21.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="43.85546875" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="21.85546875" style="2"/>
+    <col min="4" max="8" width="21.85546875" style="2"/>
+    <col min="9" max="9" width="21.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="43.85546875" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="21.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -646,425 +673,470 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>800088702</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="2">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="H2" s="2">
-        <v>23001010102</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I2" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>805001157</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="2">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="H3" s="2">
-        <v>23001010102</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I3" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>800130907</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="2">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="H4" s="2">
-        <v>23001010102</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I4" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>800251440</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="2">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="H5" s="2">
-        <v>23001010102</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I5" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>900156264</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="2">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="H6" s="2">
-        <v>23001010102</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I6" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>809008362</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="2">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="H7" s="2">
-        <v>23001010102</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I7" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>900935126</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="2">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="H8" s="2">
-        <v>23001010102</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I8" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>860066942</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="2">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="H9" s="2">
-        <v>23001010102</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I9" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>890303093</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="2">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="H10" s="2">
-        <v>23001010102</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I10" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>830003564</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="2">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="H11" s="2">
-        <v>23001010102</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I11" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>901037916</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="2">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="H12" s="2">
-        <v>23001010102</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I12" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>900226715</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="2">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="H13" s="2">
-        <v>23001010102</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I13" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>900226715</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="2">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="H14" s="2">
-        <v>23001010102</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I14" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>900336004</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="2">
+      <c r="G15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" s="2">
         <v>74</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>23001010201</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>800229739</v>
       </c>
@@ -1072,28 +1144,31 @@
         <v>230201</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="2">
+      <c r="G16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H16" s="2">
         <v>74</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>23001010201</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>800227940</v>
       </c>
@@ -1101,28 +1176,31 @@
         <v>231001</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="2">
+      <c r="G17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17" s="2">
         <v>74</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <v>23001010201</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>800224808</v>
       </c>
@@ -1130,315 +1208,348 @@
         <v>230301</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="2">
+      <c r="G18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="2">
         <v>74</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I18" s="2">
         <v>23001010201</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>860011153</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="2">
+        <v>25</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" s="2">
         <v>89</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I19" s="2">
         <v>23001010301</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>891480000</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" s="2">
+        <v>26</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="2">
         <v>75</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I20" s="2">
         <v>23001010401</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>899999239</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21" s="2">
+        <v>28</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H21" s="2">
         <v>76</v>
       </c>
-      <c r="H21" s="2">
+      <c r="I21" s="2">
         <v>230010108</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>899999034</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" s="2">
+        <v>29</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" s="2">
         <v>77</v>
       </c>
-      <c r="H22" s="2">
+      <c r="I22" s="2">
         <v>230010105</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>899999054</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G23" s="2">
+        <v>30</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H23" s="2">
         <v>72</v>
       </c>
-      <c r="H23" s="2">
+      <c r="I23" s="2">
         <v>230010106</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>899999001</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G24" s="2">
+        <v>31</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H24" s="2">
         <v>90</v>
       </c>
-      <c r="H24" s="2">
+      <c r="I24" s="2">
         <v>230010107</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>901097473</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" s="2">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="H25" s="2">
-        <v>23001010102</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I25" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>805000427</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" s="2">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="H26" s="2">
-        <v>23001010102</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I26" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>814000337</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" s="2">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="H27" s="2">
-        <v>23001010102</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="I27" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>800140949</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" s="2">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="H28" s="2">
-        <v>23001010102</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
+      </c>
+      <c r="I28" s="2">
+        <v>23001010102</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>